<commit_message>
Finished Project and added finishing touches. Also updated Reaper project as it was out of date
</commit_message>
<xml_diff>
--- a/documentation/Final_Asset_List.xlsx
+++ b/documentation/Final_Asset_List.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="57">
   <si>
     <t>Filename</t>
   </si>
@@ -28,60 +28,66 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Background Level</t>
+    <t>Level Switch</t>
+  </si>
+  <si>
+    <t>FX</t>
+  </si>
+  <si>
+    <t>The sound when the player switches to the next level</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Player Move</t>
+  </si>
+  <si>
+    <t>The player walking</t>
+  </si>
+  <si>
+    <t>Zombie Move</t>
+  </si>
+  <si>
+    <t>The enemies walking</t>
+  </si>
+  <si>
+    <t>Zombie Attack</t>
+  </si>
+  <si>
+    <t>When the enemies attack the player</t>
+  </si>
+  <si>
+    <t>Food Crunch</t>
+  </si>
+  <si>
+    <t>When the player picks up a food item</t>
+  </si>
+  <si>
+    <t>Created two new sounds for the food and drink as the single sound didn't fit with the astetic in my opinion</t>
+  </si>
+  <si>
+    <t>Soda Drink</t>
+  </si>
+  <si>
+    <t>When the player picks up a drink item</t>
+  </si>
+  <si>
+    <t>^^^^^</t>
+  </si>
+  <si>
+    <t>Hit Wall</t>
+  </si>
+  <si>
+    <t>When the player hits/runs into a wall</t>
+  </si>
+  <si>
+    <t>Game Over</t>
   </si>
   <si>
     <t>Music</t>
   </si>
   <si>
-    <t>The background track that plays during the main game loop</t>
-  </si>
-  <si>
-    <t>In Progress</t>
-  </si>
-  <si>
-    <t>Level Switch</t>
-  </si>
-  <si>
-    <t>FX</t>
-  </si>
-  <si>
-    <t>The sound when the player switches to the next level</t>
-  </si>
-  <si>
-    <t>Player Move</t>
-  </si>
-  <si>
-    <t>The player walking</t>
-  </si>
-  <si>
-    <t>Zombie Move</t>
-  </si>
-  <si>
-    <t>The enemies walking</t>
-  </si>
-  <si>
-    <t>Zombie Attack</t>
-  </si>
-  <si>
-    <t>When the enemies attack the player</t>
-  </si>
-  <si>
-    <t>Pickup Food</t>
-  </si>
-  <si>
-    <t>When the player picks up food</t>
-  </si>
-  <si>
-    <t>Hit Wall</t>
-  </si>
-  <si>
-    <t>When the player hits/runs into a wall</t>
-  </si>
-  <si>
-    <t>Game Over</t>
-  </si>
-  <si>
     <t>The track that plays when the player runs out of food</t>
   </si>
   <si>
@@ -115,7 +121,7 @@
     <t>An ambient track that plays as the player traverses the levels</t>
   </si>
   <si>
-    <t>Could also be combined with Background Level</t>
+    <t>(Would like to do a rework before the final submission)</t>
   </si>
   <si>
     <t>Player Death</t>
@@ -127,6 +133,21 @@
     <t>Can play off of Game Over</t>
   </si>
   <si>
+    <t>Proximiy to Enemies</t>
+  </si>
+  <si>
+    <t>A sound that plays when the player gets in a certain range of the enemy</t>
+  </si>
+  <si>
+    <t>Paramaterized</t>
+  </si>
+  <si>
+    <t>Enter Exit</t>
+  </si>
+  <si>
+    <t>The sound when the player enters the exit</t>
+  </si>
+  <si>
     <t>Enemy Death</t>
   </si>
   <si>
@@ -139,6 +160,9 @@
     <t>Whenever the player hits the enemy</t>
   </si>
   <si>
+    <t>Will likely change as the sound does not quite fit</t>
+  </si>
+  <si>
     <t>Menu Interface</t>
   </si>
   <si>
@@ -155,6 +179,9 @@
   </si>
   <si>
     <t>The music that plays during the main menu screen</t>
+  </si>
+  <si>
+    <t>In but would like to lengthen</t>
   </si>
 </sst>
 </file>
@@ -174,16 +201,16 @@
     </font>
     <font>
       <sz val="12.0"/>
-      <name val="Nunito"/>
-    </font>
-    <font>
-      <sz val="12.0"/>
       <color rgb="FF000000"/>
       <name val="Nunito"/>
     </font>
     <font>
       <sz val="12.0"/>
       <color theme="1"/>
+      <name val="Nunito"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
       <name val="Nunito"/>
     </font>
   </fonts>
@@ -230,7 +257,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="13">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -246,40 +273,72 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE8B2"/>
+          <bgColor rgb="FFFCE8B2"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
@@ -304,7 +363,7 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4285F4"/>
+        <a:srgbClr val="78A9FB"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="EA4335"/>
@@ -495,7 +554,7 @@
     <col customWidth="1" min="2" max="2" width="16.86"/>
     <col customWidth="1" min="3" max="3" width="81.14"/>
     <col customWidth="1" min="4" max="4" width="14.43"/>
-    <col customWidth="1" min="5" max="5" width="53.71"/>
+    <col customWidth="1" min="5" max="5" width="106.14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -519,347 +578,412 @@
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="5"/>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="6"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="4" t="s">
+      <c r="B4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="7"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="4" t="s">
+      <c r="B5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="7"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="7"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="4" t="s">
+      <c r="B6" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="7"/>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="4" t="s">
+      <c r="B7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="7"/>
+      <c r="D7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="6"/>
+      <c r="B8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="5"/>
     </row>
     <row r="9">
-      <c r="A9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="6"/>
+      <c r="B9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="5"/>
     </row>
     <row r="10">
-      <c r="A10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="3" t="s">
+      <c r="A10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="7"/>
     </row>
     <row r="11">
-      <c r="A11" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="3" t="s">
+      <c r="A11" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E11" s="7"/>
     </row>
     <row r="12">
       <c r="A12" s="8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="10"/>
+        <v>32</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="9"/>
     </row>
     <row r="13">
       <c r="A13" s="8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="11" t="s">
-        <v>38</v>
+      <c r="A15" s="8" t="s">
+        <v>40</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="10"/>
+        <v>41</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="16">
-      <c r="A16" s="11" t="s">
-        <v>40</v>
+      <c r="A16" s="8" t="s">
+        <v>43</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="10"/>
+        <v>44</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="9"/>
     </row>
     <row r="17">
-      <c r="A17" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="14"/>
+      <c r="A17" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="9"/>
     </row>
     <row r="18">
-      <c r="A18" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="6"/>
+      <c r="A18" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="19">
-      <c r="A19" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="14"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="14"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="14"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
+      <c r="A19" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="8"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="5"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="24">
-      <c r="A24" s="14"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
+      <c r="A24" s="12"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
     </row>
     <row r="25">
-      <c r="A25" s="14"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
+      <c r="A25" s="12"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
     </row>
     <row r="26">
-      <c r="A26" s="14"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
+      <c r="A26" s="12"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
     </row>
     <row r="27">
-      <c r="A27" s="14"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
+      <c r="A27" s="12"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
     </row>
     <row r="28">
-      <c r="A28" s="14"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
+      <c r="A28" s="12"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
     </row>
     <row r="29">
-      <c r="A29" s="14"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
+      <c r="A29" s="12"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
     </row>
     <row r="30">
-      <c r="A30" s="14"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
+      <c r="A30" s="12"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
     </row>
     <row r="31">
-      <c r="A31" s="14"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
+      <c r="A31" s="12"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="12"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="12"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A2:C5 D2:D21 E2:E5 A8:C14 E8:E14 A17:C21 E17:E21">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="In Reaper">
+      <formula>NOT(ISERROR(SEARCH(("In Reaper"),(A2))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:C5 D2:D21 E2:E5 A8:C14 E8:E14 A17:C21 E17:E21">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="In FMOD">
+      <formula>NOT(ISERROR(SEARCH(("In FMOD"),(A2))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:C5 D2:D21 E2:E5 A8:C14 E8:E14 A17:C21 E17:E21">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Completed">
+      <formula>NOT(ISERROR(SEARCH(("Completed"),(A2))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D21">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="In Game">
+      <formula>NOT(ISERROR(SEARCH(("In Game"),(D2))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="5">
+      <formula>LEN(TRIM(D16))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>